<commit_message>
fix Trypan blue config
</commit_message>
<xml_diff>
--- a/enmconvertor/src/main/resources/net/enanomapper/templates/INVITRO/VIABILITY/TrypanBlue/INVITRO_VIABILITY_Trypan blue_COLUMNS.xlsx
+++ b/enmconvertor/src/main/resources/net/enanomapper/templates/INVITRO/VIABILITY/TrypanBlue/INVITRO_VIABILITY_Trypan blue_COLUMNS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="555" windowWidth="22695" windowHeight="13995" activeTab="1"/>
+    <workbookView xWindow="630" yWindow="555" windowWidth="22695" windowHeight="13995"/>
   </bookViews>
   <sheets>
     <sheet name="instruction for data logging" sheetId="1" r:id="rId1"/>
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>SAMPLE INFORMATION</t>
   </si>
@@ -423,75 +423,9 @@
     <t>References to sops</t>
   </si>
   <si>
-    <t>test_a6</t>
-  </si>
-  <si>
-    <t>test_b6</t>
-  </si>
-  <si>
-    <t>test_c6</t>
-  </si>
-  <si>
-    <t>123-45-6</t>
-  </si>
-  <si>
-    <t>test_e6</t>
-  </si>
-  <si>
-    <t>test_f6</t>
-  </si>
-  <si>
-    <t>test_i6</t>
-  </si>
-  <si>
-    <t>test_j</t>
-  </si>
-  <si>
-    <t>test_k</t>
-  </si>
-  <si>
-    <t>test_l</t>
-  </si>
-  <si>
-    <t>test_m</t>
-  </si>
-  <si>
-    <t>test_n</t>
-  </si>
-  <si>
-    <t>cell viability</t>
-  </si>
-  <si>
-    <t>trypan blue</t>
-  </si>
-  <si>
-    <t>test_r6</t>
-  </si>
-  <si>
-    <t>test_s6</t>
-  </si>
-  <si>
-    <t>test_t6</t>
-  </si>
-  <si>
-    <t>test_u6</t>
-  </si>
-  <si>
-    <t>test_y6</t>
-  </si>
-  <si>
     <t>PDI</t>
   </si>
   <si>
-    <t>test_ab6</t>
-  </si>
-  <si>
-    <t>test_ad6</t>
-  </si>
-  <si>
-    <t>test_ae6</t>
-  </si>
-  <si>
     <t>µg/ml</t>
   </si>
   <si>
@@ -502,12 +436,6 @@
   </si>
   <si>
     <t>sd</t>
-  </si>
-  <si>
-    <t>test-ak6</t>
-  </si>
-  <si>
-    <t>test_aq6</t>
   </si>
 </sst>
 </file>
@@ -1637,6 +1565,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1660,11 +1593,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1677,6 +1605,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>37464</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>133739</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9791064" cy="13278239"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1966,282 +1937,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AQ7"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="42" max="42" width="9.5703125" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AP2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="Z3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AH5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" t="s">
-        <v>55</v>
-      </c>
-      <c r="K6" t="s">
-        <v>56</v>
-      </c>
-      <c r="L6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M6" t="s">
-        <v>58</v>
-      </c>
-      <c r="N6" t="s">
-        <v>59</v>
-      </c>
-      <c r="P6" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>61</v>
-      </c>
-      <c r="R6" t="s">
-        <v>62</v>
-      </c>
-      <c r="S6" t="s">
-        <v>63</v>
-      </c>
-      <c r="T6" t="s">
-        <v>64</v>
-      </c>
-      <c r="U6" t="s">
-        <v>65</v>
-      </c>
-      <c r="V6">
-        <v>1.23</v>
-      </c>
-      <c r="W6">
-        <v>2.34</v>
-      </c>
-      <c r="X6">
-        <v>3.45</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z6">
-        <v>7.77</v>
-      </c>
-      <c r="AA6">
-        <v>1</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC6">
-        <v>1</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF6">
-        <v>10</v>
-      </c>
-      <c r="AG6">
-        <v>7</v>
-      </c>
-      <c r="AH6">
-        <v>3.14</v>
-      </c>
-      <c r="AI6">
-        <v>4.25</v>
-      </c>
-      <c r="AJ6">
-        <v>2</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL6">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="AM6">
-        <v>10</v>
-      </c>
-      <c r="AN6">
-        <v>5.55</v>
-      </c>
-      <c r="AO6">
-        <v>56.7</v>
-      </c>
-      <c r="AP6">
-        <v>1.8</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" t="s">
-        <v>58</v>
-      </c>
-      <c r="N7" t="s">
-        <v>59</v>
-      </c>
-      <c r="P7" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>61</v>
-      </c>
-      <c r="R7" t="s">
-        <v>62</v>
-      </c>
-      <c r="S7" t="s">
-        <v>63</v>
-      </c>
-      <c r="T7" t="s">
-        <v>64</v>
-      </c>
-      <c r="U7" t="s">
-        <v>65</v>
-      </c>
-      <c r="V7">
-        <v>1.23</v>
-      </c>
-      <c r="W7">
-        <v>2.34</v>
-      </c>
-      <c r="X7">
-        <v>3.45</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z7">
-        <v>7.77</v>
-      </c>
-      <c r="AA7">
-        <v>1</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC7">
-        <v>1</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF7">
-        <v>10</v>
-      </c>
-      <c r="AG7">
-        <v>7</v>
-      </c>
-      <c r="AH7">
-        <v>3.14</v>
-      </c>
-      <c r="AI7">
-        <v>4.25</v>
-      </c>
-      <c r="AJ7">
-        <v>2</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL7">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="AM7">
-        <v>10</v>
-      </c>
-      <c r="AN7">
-        <v>5.55</v>
-      </c>
-      <c r="AO7">
-        <v>56.7</v>
-      </c>
-      <c r="AP7">
-        <v>1.8</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2249,7 +1955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -2301,55 +2007,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="765" t="s">
+      <c r="A1" s="768" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="766"/>
-      <c r="C1" s="766"/>
-      <c r="D1" s="766"/>
-      <c r="E1" s="766"/>
-      <c r="F1" s="766"/>
-      <c r="G1" s="766"/>
-      <c r="H1" s="766"/>
-      <c r="I1" s="766"/>
-      <c r="J1" s="766"/>
-      <c r="K1" s="766"/>
-      <c r="L1" s="766"/>
-      <c r="M1" s="766"/>
-      <c r="N1" s="767"/>
-      <c r="O1" s="769"/>
-      <c r="P1" s="770"/>
-      <c r="Q1" s="771"/>
-      <c r="R1" s="775" t="s">
+      <c r="B1" s="769"/>
+      <c r="C1" s="769"/>
+      <c r="D1" s="769"/>
+      <c r="E1" s="769"/>
+      <c r="F1" s="769"/>
+      <c r="G1" s="769"/>
+      <c r="H1" s="769"/>
+      <c r="I1" s="769"/>
+      <c r="J1" s="769"/>
+      <c r="K1" s="769"/>
+      <c r="L1" s="769"/>
+      <c r="M1" s="769"/>
+      <c r="N1" s="770"/>
+      <c r="O1" s="772"/>
+      <c r="P1" s="773"/>
+      <c r="Q1" s="774"/>
+      <c r="R1" s="778" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="776"/>
-      <c r="T1" s="776"/>
-      <c r="U1" s="776"/>
-      <c r="V1" s="776"/>
-      <c r="W1" s="776"/>
-      <c r="X1" s="776"/>
-      <c r="Y1" s="776"/>
-      <c r="Z1" s="776"/>
-      <c r="AA1" s="777"/>
-      <c r="AB1" s="772"/>
-      <c r="AC1" s="773"/>
-      <c r="AD1" s="773"/>
-      <c r="AE1" s="773"/>
-      <c r="AF1" s="773"/>
-      <c r="AG1" s="773"/>
-      <c r="AH1" s="773"/>
-      <c r="AI1" s="773"/>
-      <c r="AJ1" s="773"/>
-      <c r="AK1" s="773"/>
-      <c r="AL1" s="773"/>
-      <c r="AM1" s="774"/>
-      <c r="AN1" s="769" t="s">
+      <c r="S1" s="779"/>
+      <c r="T1" s="779"/>
+      <c r="U1" s="779"/>
+      <c r="V1" s="779"/>
+      <c r="W1" s="779"/>
+      <c r="X1" s="779"/>
+      <c r="Y1" s="779"/>
+      <c r="Z1" s="779"/>
+      <c r="AA1" s="780"/>
+      <c r="AB1" s="775"/>
+      <c r="AC1" s="776"/>
+      <c r="AD1" s="776"/>
+      <c r="AE1" s="776"/>
+      <c r="AF1" s="776"/>
+      <c r="AG1" s="776"/>
+      <c r="AH1" s="776"/>
+      <c r="AI1" s="776"/>
+      <c r="AJ1" s="776"/>
+      <c r="AK1" s="776"/>
+      <c r="AL1" s="776"/>
+      <c r="AM1" s="777"/>
+      <c r="AN1" s="772" t="s">
         <v>42</v>
       </c>
-      <c r="AO1" s="770"/>
-      <c r="AP1" s="771"/>
-      <c r="AQ1" s="768" t="s">
+      <c r="AO1" s="773"/>
+      <c r="AP1" s="774"/>
+      <c r="AQ1" s="771" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2405,18 +2111,18 @@
       <c r="Q2" s="273" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="778" t="s">
+      <c r="R2" s="765" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="779"/>
-      <c r="T2" s="779"/>
-      <c r="U2" s="779"/>
-      <c r="V2" s="779"/>
-      <c r="W2" s="779"/>
-      <c r="X2" s="779"/>
-      <c r="Y2" s="779"/>
-      <c r="Z2" s="779"/>
-      <c r="AA2" s="780"/>
+      <c r="S2" s="766"/>
+      <c r="T2" s="766"/>
+      <c r="U2" s="766"/>
+      <c r="V2" s="766"/>
+      <c r="W2" s="766"/>
+      <c r="X2" s="766"/>
+      <c r="Y2" s="766"/>
+      <c r="Z2" s="766"/>
+      <c r="AA2" s="767"/>
       <c r="AB2" s="55" t="s">
         <v>30</v>
       </c>
@@ -2460,7 +2166,7 @@
         <v>44</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="AQ2" s="747" t="s">
         <v>47</v>
@@ -2509,7 +2215,7 @@
         <v>29</v>
       </c>
       <c r="Z3" s="333" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="AA3" s="334" t="s">
         <v>29</v>
@@ -2617,17 +2323,17 @@
       <c r="AF5" s="95"/>
       <c r="AG5" s="96"/>
       <c r="AH5" s="97" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="AI5" s="98" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="AJ5" s="99" t="s">
         <v>26</v>
       </c>
       <c r="AK5" s="100"/>
       <c r="AL5" s="101" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="AM5" s="102"/>
       <c r="AN5" s="10"/>

</xml_diff>